<commit_message>
Refactoring code. Add Bridge Damage Summarys
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/桥梁病害汇总表.xlsx
+++ b/AutoRegularInspection/桥梁病害汇总表.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649053DF-FCE1-4E50-BF4F-38547145B722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F922A050-BF31-49CB-B35A-DCC3CEDC3FA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="1710" windowWidth="16485" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
+    <sheet name="上部结构" sheetId="2" r:id="rId2"/>
+    <sheet name="下部结构" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="93">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -204,6 +206,161 @@
   <si>
     <t>残缺</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主梁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>表面裂缝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>混凝土剥离</t>
+  </si>
+  <si>
+    <t>混凝土剥离</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>露筋锈蚀</t>
+  </si>
+  <si>
+    <t>梁体下挠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>结构裂缝</t>
+  </si>
+  <si>
+    <t>结构裂缝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>裂缝处渗水</t>
+  </si>
+  <si>
+    <t>裂缝处渗水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桥面贯通横缝</t>
+  </si>
+  <si>
+    <t>梁体位移</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横向联系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>桥面贯通纵缝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连接件脱焊松动</t>
+  </si>
+  <si>
+    <t>连接件断裂</t>
+  </si>
+  <si>
+    <t>连接件断裂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横隔板网裂</t>
+  </si>
+  <si>
+    <t>横隔板网裂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横隔板剥落露筋</t>
+  </si>
+  <si>
+    <t>横隔板剥落露筋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>梁体异常振动</t>
+  </si>
+  <si>
+    <t>梁体异常振动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防落梁装置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有无落架趋势</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>牛腿表面损伤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伸缩缝处渗水</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钢锚板锈蚀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>台帽</t>
+  </si>
+  <si>
+    <t>墩台成块剥落</t>
+  </si>
+  <si>
+    <t>盖梁</t>
+  </si>
+  <si>
+    <t>墩身</t>
+  </si>
+  <si>
+    <t>墩身水平裂缝</t>
+  </si>
+  <si>
+    <t>墩身纵向裂缝</t>
+  </si>
+  <si>
+    <t>框架式节点裂缝</t>
+  </si>
+  <si>
+    <t>桥墩倾斜</t>
+  </si>
+  <si>
+    <t>台身</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耳背翼墙</t>
+  </si>
+  <si>
+    <t>支座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固定螺栓损坏</t>
+  </si>
+  <si>
+    <t>橡胶支座变形</t>
+  </si>
+  <si>
+    <t>钢支座损坏</t>
+  </si>
+  <si>
+    <t>底板混凝土破损</t>
+  </si>
+  <si>
+    <t>稳定性异常</t>
+  </si>
+  <si>
+    <t>钢垫板锈蚀</t>
   </si>
 </sst>
 </file>
@@ -530,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1580,4 +1737,1631 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16F47B95-C7A3-4623-A36A-AB1202BB73A7}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE83029-A805-4535-A6D5-DF10F8642D4E}">
+  <dimension ref="A1:G46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+      <c r="E25" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+      <c r="D29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29">
+        <v>5</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40">
+        <v>5</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42">
+        <v>5</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>67</v>
+      </c>
+      <c r="F43">
+        <v>4</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>69</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>6</v>
+      </c>
+      <c r="G45">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
divide Severity into SeverityQuantity and SeverityQuality
</commit_message>
<xml_diff>
--- a/AutoRegularInspection/桥梁病害汇总表.xlsx
+++ b/AutoRegularInspection/桥梁病害汇总表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eamdf\source\repos\AutoRegularInspection\AutoRegularInspection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4433C6A6-A005-41D6-A6D9-367BD9B1325D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB33B7F-F3AB-40DC-877F-9E1339AD77E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="2160" windowWidth="24360" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="桥面系" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>